<commit_message>
xlsx needs to be turned into a csv or json to avoid git bloat
</commit_message>
<xml_diff>
--- a/log_analyzer/log_messages.xlsx
+++ b/log_analyzer/log_messages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hbreaux\Documents\Programs\Test Programs\Log Parser v2\Cradlepoint-Log-Parser\log_analyzer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B12356E-3D21-4A53-BB60-870C295E7C8D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{444766EE-77BE-4655-AE96-86A81A1D2EEB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11325" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -148,7 +148,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="60">
   <si>
     <t>This database is meant to serve as a repository of common log messages and their meanings.  Log messages must always be interpreted in the context of what is around them.  This database is not meant to be a replacement for troubleshooting and it is not intended to interpret logs for you.  This repository has been designed as an assistant to help engineers work with logs more effeciently.  Anyone using it must be careful not to let it act as a replacement for their own critical thinking and reasoning skills. </t>
   </si>
@@ -325,6 +325,9 @@
   </si>
   <si>
     <t>Recieved a notifcation from the other side of the tunnel that setup of Phase 2 Child SAs(security associations) failed. This failure is usually due to a local/remote traffic selector mismatch, or some other phase 2 encryption/hash/algorithm mismatch.  Log messages above this can help give context to what caused the failure.   https://customer.cradlepoint.com/s/article/Local-Network-Mismatch-Policy-Based-IPSec-VPN-NCOS-7-0-40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INFO, IPSEC CFG: 2, IKE: 2 </t>
   </si>
 </sst>
 </file>
@@ -1161,7 +1164,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1260,7 +1263,7 @@
     </row>
     <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B6" s="17" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
Improved regex in log_messages.xlsx to be more specific
</commit_message>
<xml_diff>
--- a/log_analyzer/log_messages.xlsx
+++ b/log_analyzer/log_messages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hbreaux\Documents\Programs\Test Programs\Log Parser v2\Cradlepoint-Log-Parser\log_analyzer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{444766EE-77BE-4655-AE96-86A81A1D2EEB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F84AC65-3B57-43E0-B6C2-1D1202C6B432}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11325" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -148,7 +148,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="58">
   <si>
     <t>This database is meant to serve as a repository of common log messages and their meanings.  Log messages must always be interpreted in the context of what is around them.  This database is not meant to be a replacement for troubleshooting and it is not intended to interpret logs for you.  This repository has been designed as an assistant to help engineers work with logs more effeciently.  Anyone using it must be careful not to let it act as a replacement for their own critical thinking and reasoning skills. </t>
   </si>
@@ -186,48 +186,24 @@
     <t>WAN</t>
   </si>
   <si>
-    <t>These message appear peridoically in the log of a Cradlepoint with a modem.  The values in them indicate the signal strength of the modem.  Look at the timestamp to determine what time the signal strength information is from.  If youre running into intermittent connectivity issues, check these message to see if you have poor signal strength.  See this article for help interpretting whether your signal strength values are good or poor: https://customer.cradlepoint.com/s/article/Modem-Signal-Strength-and-Signal-Quality</t>
-  </si>
-  <si>
     <t>ERROR</t>
   </si>
   <si>
-    <t>WAN:.*.CPPM|Connect Error</t>
-  </si>
-  <si>
     <t>CPPM Connect Errors indicate the modem had an issue connecting to the carrier.  If you look after this Connect Error message the logs should show the specific error.  This article has more information on common connect error messages: https://customer.cradlepoint.com/s/article/NCOS-No-Internet-or-Connection-Issues</t>
   </si>
   <si>
-    <t>WAN:.*.CPPM|state=connecting  result=carrier reject</t>
-  </si>
-  <si>
     <t>The modem tried to connect but failed because of a carrier reject.  Carrier reject usually indicates improper provisioning from the carrier or the wrong APN is being used.  </t>
   </si>
   <si>
-    <t>WAN:.*|Connect Event: carrier reject - state: connecting</t>
-  </si>
-  <si>
     <t>cp_stack_mgr</t>
   </si>
   <si>
-    <t>cp_stack_mgr|modem.*: LTE Modem data connection failed - status:26</t>
-  </si>
-  <si>
     <t>The LTE connection to the internet failed.  Status 26 indicates a carrier reject event.  Carrier reject is usually a result of improper provisioning from the carrier or the wrong APN being used.  </t>
   </si>
   <si>
-    <t>WAN:.*.CPPM|state=connecting  result=no carrier</t>
-  </si>
-  <si>
     <t xml:space="preserve">No carrier is an error that typically indicates bad provisioning by the carrier.  In some cases it can also appear if the modem is in an area with very poor signal strength.  To resolve this error you usually want to verify provisioning with the carrier and/or move the modem to an area with better signal strength. </t>
   </si>
   <si>
-    <t>WAN:.*|Connect Event: no carrier - state: connecting </t>
-  </si>
-  <si>
-    <t>.*: LTE Modem data connection failed - status:9 </t>
-  </si>
-  <si>
     <t xml:space="preserve">The LTE connection to the internet failed.  Status 9 indicates a no carrier error.  No carrier is usually a result of bad provisioning or very poor signal strength.  </t>
   </si>
   <si>
@@ -249,9 +225,6 @@
     <t>Problematic</t>
   </si>
   <si>
-    <t>WAN:.*|SIM error: NOSIM</t>
-  </si>
-  <si>
     <t>WARN</t>
   </si>
   <si>
@@ -270,9 +243,6 @@
     <t>state=connecting result=unknown error</t>
   </si>
   <si>
-    <t>WAN:.*| signal .* (S.*) on port modem1: .*%, RSSI:-.*(dBm), SINR:.*(dB), RSRP:-.*(dB), RSRQ:-.*(dB), RFBAND: Band .*</t>
-  </si>
-  <si>
     <t xml:space="preserve">A CPPM unknown error usually indicates the modem or SIM is not functioning properly.  It can also indicate modem/SIM card provisioning errors.  </t>
   </si>
   <si>
@@ -285,15 +255,9 @@
     <t>IPSEC</t>
   </si>
   <si>
-    <t>generating IKE_AUTH response 1 [ N(AUTH_FAILED) ]</t>
-  </si>
-  <si>
     <t>IPSec peer failed authentication, and an AUTH_FAILED response is being sent to it.  This can often times mean there is a pre-shared key mismatch.  https://customer.cradlepoint.com/s/article/Pre-Shared-Key-Mismatch-Policy-Based-IPSec-VPN-NCOS-7-0-40</t>
   </si>
   <si>
-    <t>parsed IKE_AUTH response 1 [ N(AUTH_FAILED) ]</t>
-  </si>
-  <si>
     <t>IPSec peer failed authentication, and an AUTH_FAILED response was received.  This can often times mean there is a pre-shared key mismatch.  https://customer.cradlepoint.com/s/article/Pre-Shared-Key-Mismatch-Policy-Based-IPSec-VPN-NCOS-7-0-40</t>
   </si>
   <si>
@@ -303,9 +267,6 @@
     <t>INFO, IPSEC CFG: 2, IKE: 2</t>
   </si>
   <si>
-    <t>traffic selectors .* === .* inacceptable</t>
-  </si>
-  <si>
     <t>There is a mismatch between the local and remote networks that each side of the tunnel is proposing.  Check to ensure that each side has the correct local/remote networks configured.  https://customer.cradlepoint.com/s/article/Local-Network-Mismatch-Policy-Based-IPSec-VPN-NCOS-7-0-40</t>
   </si>
   <si>
@@ -315,9 +276,6 @@
     <t>Setup of Phase 2 Child SAs(security associations) failed.  This is usually due to a local/remote traffic selector mismatch, or some other phase 2 encryption/hash/algorithm mismatch.  Log messages above this can help give context to what caused the failure.  https://customer.cradlepoint.com/s/article/Local-Network-Mismatch-Policy-Based-IPSec-VPN-NCOS-7-0-40</t>
   </si>
   <si>
-    <t>generating IKE_AUTH response 1 [ IDr AUTH N(MOBIKE_SUP) N(ADD_4_ADDR) N(ADD_4_ADDR) N(ADD_4_ADDR) N(TS_UNACCEPT) ]</t>
-  </si>
-  <si>
     <t>Setup of Phase 2 Child SAs(security associations) failed, so a response to notify the other side of the tunnel is being generated and sent.  This failure is usually due to a local/remote traffic selector mismatch, or some other phase 2 encryption/hash/algorithm mismatch.  Log messages above this can help give context to what caused the failure.   https://customer.cradlepoint.com/s/article/Local-Network-Mismatch-Policy-Based-IPSec-VPN-NCOS-7-0-40</t>
   </si>
   <si>
@@ -328,6 +286,42 @@
   </si>
   <si>
     <t xml:space="preserve">INFO, IPSEC CFG: 2, IKE: 2 </t>
+  </si>
+  <si>
+    <t>Connect Event: no carrier - state: connecting </t>
+  </si>
+  <si>
+    <t>LTE Modem data connection failed - status:9 </t>
+  </si>
+  <si>
+    <t>SIM error: NOSIM</t>
+  </si>
+  <si>
+    <t>state=connecting  result=no carrier</t>
+  </si>
+  <si>
+    <t>LTE Modem data connection failed - status:26</t>
+  </si>
+  <si>
+    <t>Connect Event: carrier reject - state: connecting</t>
+  </si>
+  <si>
+    <t>state=connecting  result=carrier reject</t>
+  </si>
+  <si>
+    <t>Connect Error</t>
+  </si>
+  <si>
+    <t>traffic selectors \d{1,3}\.\d{1,3}\.\d{1,3}\.\d{1,3}\/\d{1,2} === \d{1,3}\.\d{1,3}\.\d{1,3}\.\d{1,3}\/\d{1,2} inacceptable</t>
+  </si>
+  <si>
+    <t>generating IKE_AUTH response 1 \[ N\(AUTH_FAILED\) \]</t>
+  </si>
+  <si>
+    <t>parsed IKE_AUTH response 1 \[ N\(AUTH_FAILED\) \]</t>
+  </si>
+  <si>
+    <t>generating IKE_AUTH response 1 \[ IDr AUTH N\(MOBIKE_SUP\) N\(ADD_4_ADDR\) N\(ADD_4_ADDR\) N\(ADD_4_ADDR\) N\(TS_UNACCEPT\) \]</t>
   </si>
 </sst>
 </file>
@@ -895,11 +889,11 @@
   <sheetPr>
     <tabColor rgb="FFFCE4D6"/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,40 +919,40 @@
         <v>9</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="15" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="E2" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="3" t="b">
+      <c r="E3" s="15" t="b">
         <v>1</v>
       </c>
     </row>
@@ -970,44 +964,44 @@
         <v>11</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E4" s="15" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" s="15" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E6" s="15" t="b">
         <v>1</v>
@@ -1021,41 +1015,41 @@
         <v>11</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E7" s="15" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="15" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="C9" s="3" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>26</v>
@@ -1066,33 +1060,33 @@
     </row>
     <row r="10" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E10" s="15" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>36</v>
+      <c r="C11" t="s">
+        <v>29</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E11" s="15" t="b">
         <v>1</v>
@@ -1106,46 +1100,29 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="E12" s="15" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C13" t="s">
-        <v>39</v>
+      <c r="C13" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E13" s="15" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" s="15" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1164,7 +1141,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1190,21 +1167,21 @@
         <v>9</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="E2" s="17" t="b">
         <v>1</v>
@@ -1212,16 +1189,16 @@
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="E3" s="17" t="b">
         <v>1</v>
@@ -1229,16 +1206,16 @@
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="E4" s="17" t="b">
         <v>1</v>
@@ -1246,16 +1223,16 @@
     </row>
     <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E5" s="17" t="b">
         <v>1</v>
@@ -1263,16 +1240,16 @@
     </row>
     <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="E6" s="17" t="b">
         <v>1</v>
@@ -1280,16 +1257,16 @@
     </row>
     <row r="7" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="E7" s="17" t="b">
         <v>1</v>
@@ -1297,16 +1274,16 @@
     </row>
     <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B8" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="17" t="s">
         <v>44</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1421,13 +1398,13 @@
         <v>10</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1435,13 +1412,13 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed file open error messagebox
</commit_message>
<xml_diff>
--- a/log_analyzer/log_messages.xlsx
+++ b/log_analyzer/log_messages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hbreaux\Documents\Programs\Test Programs\Log Parser v2\Log Parser\Cradlepoint-Log-Parser\log_analyzer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC77C995-BAFC-4AA8-BA20-F83009099574}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5759BBC4-F5A7-4A4F-B1BF-8BE6755FC830}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11325" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Disclaimer" sheetId="6" r:id="rId1"/>
@@ -148,7 +148,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="69">
   <si>
     <t>This database is meant to serve as a repository of common log messages and their meanings.  Log messages must always be interpreted in the context of what is around them.  This database is not meant to be a replacement for troubleshooting and it is not intended to interpret logs for you.  This repository has been designed as an assistant to help engineers work with logs more effeciently.  Anyone using it must be careful not to let it act as a replacement for their own critical thinking and reasoning skills. </t>
   </si>
@@ -445,7 +445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -495,6 +495,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -924,7 +925,7 @@
   </sheetPr>
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
@@ -1347,7 +1348,7 @@
   </sheetPr>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
@@ -1456,16 +1457,16 @@
   <sheetPr>
     <tabColor rgb="FFDDEBF7"/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1477,6 +1478,9 @@
       </c>
       <c r="D1" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added some openvpn lines to search for
</commit_message>
<xml_diff>
--- a/log_analyzer/log_messages.xlsx
+++ b/log_analyzer/log_messages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hbreaux\Documents\Programs\Test Programs\Log Parser v2\Log Parser\Cradlepoint-Log-Parser\log_analyzer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5759BBC4-F5A7-4A4F-B1BF-8BE6755FC830}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5133107D-A078-47ED-9B05-B62E66D14A0D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="13890" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Disclaimer" sheetId="6" r:id="rId1"/>
@@ -39,21 +39,12 @@
   <commentList>
     <comment ref="D1" authorId="0" shapeId="0" xr:uid="{2186ADD0-9FB7-4488-B052-C6252CA5D041}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">[Threaded comment]
+        <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     The meaning of a message has to be definined to the smallest scope possible.  
 What a series of messages actually means depends a lot on context, and we need to be very careful not to bake our interpretation of a group of message into the meaning for just a single one of those messages. 
 </t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -68,21 +59,12 @@
   <commentList>
     <comment ref="D1" authorId="0" shapeId="0" xr:uid="{BFEE29A8-13CA-471B-9472-50B3FC35D610}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">[Threaded comment]
+        <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     The meaning of a message has to be definined to the smallest scope possible.  
 What a series of messages actually means depends a lot on context, and we need to be very careful not to bake our interpretation of a group of message into the meaning for just a single one of those messages. 
 </t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -97,21 +79,12 @@
   <commentList>
     <comment ref="D1" authorId="0" shapeId="0" xr:uid="{C0A6BDC1-34A6-474E-98BC-D411B4294170}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">[Threaded comment]
+        <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     The meaning of a message has to be definined to the smallest scope possible.  
 What a series of messages actually means depends a lot on context, and we need to be very careful not to bake our interpretation of a group of message into the meaning for just a single one of those messages. 
 </t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -126,21 +99,12 @@
   <commentList>
     <comment ref="D1" authorId="0" shapeId="0" xr:uid="{D31F47EC-30E6-4CBF-B73C-1EDA3035D709}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">[Threaded comment]
+        <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     The meaning of a message has to be definined to the smallest scope possible.  
 What a series of messages actually means depends a lot on context, and we need to be very careful not to bake our interpretation of a group of message into the meaning for just a single one of those messages. 
 </t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -148,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="75">
   <si>
     <t>This database is meant to serve as a repository of common log messages and their meanings.  Log messages must always be interpreted in the context of what is around them.  This database is not meant to be a replacement for troubleshooting and it is not intended to interpret logs for you.  This repository has been designed as an assistant to help engineers work with logs more effeciently.  Anyone using it must be careful not to let it act as a replacement for their own critical thinking and reasoning skills. </t>
   </si>
@@ -355,6 +319,24 @@
   </si>
   <si>
     <t xml:space="preserve">There is a mismatch in dead intervals.  Make sure the hello and dead intervals match between the routers to resolve this. </t>
+  </si>
+  <si>
+    <t>comp-lzo' is present in remote config but missing in local config, remote='comp-lzo'</t>
+  </si>
+  <si>
+    <t>OPENVPN</t>
+  </si>
+  <si>
+    <t>Comp-lzo is a compression option for OpenVPN.  Cradlepoint routers do not have a way to turn on Comp-lzo.  To get the OpenVPN tunnel to connect, the remote side of the tunnel will have to turn off the comp-lzo flag in their OpenVPN config</t>
+  </si>
+  <si>
+    <t>write to TUN/TAP : Invalid argument \(code=22\)</t>
+  </si>
+  <si>
+    <t>ERR</t>
+  </si>
+  <si>
+    <t>The remote side of the OpenVPN tunnel is trying to push the comp-lzo option to the Cradlepoint.  Cradlepoints do not support using Comp-lzo, so the tunnel wont function properly.  To get the OpenVPN tunnel to connect, the remote side of the tunnel will have to turn off the comp-lzo flag in their OpenVPN config</t>
   </si>
 </sst>
 </file>
@@ -445,7 +427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -496,6 +478,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -816,16 +801,6 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D1" dT="2019-04-23T15:56:14.37" personId="{D9D9AFB3-1855-4E26-BD95-A5BCB4A7E74D}" id="{8FAD6BDE-66E6-4729-89E1-0A40CD3F24C3}">
-    <text xml:space="preserve">The meaning of a message has to be definined to the smallest scope possible.  
-What a series of messages actually means depends a lot on context, and we need to be very careful not to bake our interpretation of a group of message into the meaning for just a single one of those messages. 
-</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
-<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="D1" dT="2019-04-23T15:56:14.37" personId="{D9D9AFB3-1855-4E26-BD95-A5BCB4A7E74D}" id="{2186ADD0-9FB7-4488-B052-C6252CA5D041}">
     <text xml:space="preserve">The meaning of a message has to be definined to the smallest scope possible.  
 What a series of messages actually means depends a lot on context, and we need to be very careful not to bake our interpretation of a group of message into the meaning for just a single one of those messages. 
@@ -834,7 +809,7 @@
 </ThreadedComments>
 </file>
 
-<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="D1" dT="2019-04-23T15:56:14.37" personId="{D9D9AFB3-1855-4E26-BD95-A5BCB4A7E74D}" id="{BFEE29A8-13CA-471B-9472-50B3FC35D610}">
     <text xml:space="preserve">The meaning of a message has to be definined to the smallest scope possible.  
@@ -844,7 +819,7 @@
 </ThreadedComments>
 </file>
 
-<file path=xl/threadedComments/threadedComment4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="D1" dT="2019-04-23T15:56:14.37" personId="{D9D9AFB3-1855-4E26-BD95-A5BCB4A7E74D}" id="{C0A6BDC1-34A6-474E-98BC-D411B4294170}">
     <text xml:space="preserve">The meaning of a message has to be definined to the smallest scope possible.  
@@ -854,7 +829,7 @@
 </ThreadedComments>
 </file>
 
-<file path=xl/threadedComments/threadedComment5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/threadedComments/threadedComment4.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="D1" dT="2019-04-23T15:56:14.37" personId="{D9D9AFB3-1855-4E26-BD95-A5BCB4A7E74D}" id="{D31F47EC-30E6-4CBF-B73C-1EDA3035D709}">
     <text xml:space="preserve">The meaning of a message has to be definined to the smallest scope possible.  
@@ -925,7 +900,7 @@
   </sheetPr>
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
@@ -1185,11 +1160,11 @@
   <sheetPr>
     <tabColor rgb="FFD6DCE4"/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1332,6 +1307,34 @@
       </c>
       <c r="D8" s="16" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>